<commit_message>
Added the ability to include snow properties as a function of time. Updated documentation. Removed checking for updates (now using github)
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>Thermal Conductivity (k)</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>(%)</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>0.1 - 0.005*t</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1040,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1131,8 +1137,8 @@
       <c r="B5" s="3">
         <v>130</v>
       </c>
-      <c r="C5" s="3">
-        <v>6.3250000000000001E-2</v>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="3">
         <v>2036</v>
@@ -1152,8 +1158,8 @@
       <c r="B6" s="3">
         <v>150</v>
       </c>
-      <c r="C6" s="3">
-        <v>0.05</v>
+      <c r="C6" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D6" s="3">
         <v>2036</v>
@@ -1358,7 +1364,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Added the ability to include snow properties as a function of time.
</commit_message>
<xml_diff>
--- a/template.xlsx
+++ b/template.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="72">
   <si>
     <t>Thermal Conductivity (k)</t>
   </si>
@@ -399,6 +399,12 @@
   </si>
   <si>
     <t>(%)</t>
+  </si>
+  <si>
+    <t>auto</t>
+  </si>
+  <si>
+    <t>0.1 - 0.005*t</t>
   </si>
 </sst>
 </file>
@@ -1034,7 +1040,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1131,8 +1137,8 @@
       <c r="B5" s="3">
         <v>130</v>
       </c>
-      <c r="C5" s="3">
-        <v>6.3250000000000001E-2</v>
+      <c r="C5" s="3" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="3">
         <v>2036</v>
@@ -1152,8 +1158,8 @@
       <c r="B6" s="3">
         <v>150</v>
       </c>
-      <c r="C6" s="3">
-        <v>0.05</v>
+      <c r="C6" s="3" t="s">
+        <v>71</v>
       </c>
       <c r="D6" s="3">
         <v>2036</v>
@@ -1358,7 +1364,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>